<commit_message>
Update the Excel format
</commit_message>
<xml_diff>
--- a/Web platform/assets/exemple.xlsx
+++ b/Web platform/assets/exemple.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yassine\Desktop\PFE_Repository\Web platform\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3730D6FE-49D4-43D0-A4FF-4F54B1C960B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593AB1D7-2892-498E-A021-49EBB58E2A49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{1654E604-2030-4D65-8EA8-B037148D8204}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Capteur</t>
-  </si>
-  <si>
-    <t>Valeur</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -43,13 +37,31 @@
   </si>
   <si>
     <t>Statistiques exportés depuis le plateforme          Data Logger v1.0</t>
+  </si>
+  <si>
+    <t>Courant DC</t>
+  </si>
+  <si>
+    <t>Tension DC</t>
+  </si>
+  <si>
+    <t>Courant AC</t>
+  </si>
+  <si>
+    <t>Température</t>
+  </si>
+  <si>
+    <t>Luminosité</t>
+  </si>
+  <si>
+    <t>Humidité</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,13 +85,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -95,7 +100,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -144,6 +149,17 @@
       <left style="thick">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thick">
         <color auto="1"/>
       </right>
@@ -153,28 +169,43 @@
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -207,15 +238,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>523876</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>207671</xdr:rowOff>
+      <xdr:rowOff>140996</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -244,8 +275,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="38100" y="238125"/>
-          <a:ext cx="6657975" cy="502946"/>
+          <a:off x="523876" y="66675"/>
+          <a:ext cx="8743950" cy="607721"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -554,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7753D55B-2905-4F4A-9530-E0E105168327}">
-  <dimension ref="B5:J11"/>
+  <dimension ref="B5:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:I7"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -565,72 +596,112 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+    <row r="5" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+    <row r="6" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+    <row r="7" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:10" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:15" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4"/>
       <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="4"/>
+      <c r="N10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="2:10" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:15" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="C5:I7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="B10:D10"/>
+  <mergeCells count="10">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="F5:L6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>